<commit_message>
Updated/Added files after scrum
</commit_message>
<xml_diff>
--- a/docs/Getana_Deliverable_2_DailyScrumReport.xlsx
+++ b/docs/Getana_Deliverable_2_DailyScrumReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="75">
   <si>
     <t>Daily Scrum Report — Sprint 1</t>
   </si>
@@ -221,6 +221,36 @@
   </si>
   <si>
     <t>What they will do: What they will do: Attend next meeting 2/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What impediments prevent them from progressing: N/A </t>
+  </si>
+  <si>
+    <t>What they have done: Attended meeting, planned presentation, planned sprint 2 product implementation</t>
+  </si>
+  <si>
+    <t>What they have done: Attended meeting, planned presentation, planned sprint 2 product implementation, updated zenhub board, updated sprint backlog</t>
+  </si>
+  <si>
+    <t>What they have done: Absent from meeting (with valid reason)</t>
+  </si>
+  <si>
+    <t>What they will do: Create user interface for creating a schedule, adding classes, and saving a schedule</t>
+  </si>
+  <si>
+    <t>What they will do: Organize focus group participants and meeting time, Create user interface for recalling schedules, schedule selection, and detail display</t>
+  </si>
+  <si>
+    <t>What they will do: Implement backend functionality for saving and recalling saved schedules</t>
+  </si>
+  <si>
+    <t>What they will do: Implement data structure for mapping building prefixes to physical addresses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What will they do: Implement driver code to utilize google maps API to generate route from provided schedule detail </t>
+  </si>
+  <si>
+    <t>What they will do: Implement front end for route display after API calls to generate route</t>
   </si>
 </sst>
 </file>
@@ -662,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="140" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView topLeftCell="A79" zoomScale="140" zoomScaleNormal="68" workbookViewId="0">
       <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
@@ -1391,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="125" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1563,17 +1593,17 @@
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C36" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C37" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.15">
@@ -1581,17 +1611,17 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C40" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C41" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.15">
@@ -1599,17 +1629,17 @@
         <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C44" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C45" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.15">
@@ -1617,17 +1647,17 @@
         <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C48" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C49" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.15">
@@ -1635,17 +1665,17 @@
         <v>20</v>
       </c>
       <c r="C51" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C52" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C53" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.15">
@@ -1653,17 +1683,17 @@
         <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C56" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C57" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Updated Scrum report, added deliverable 2 tasks word document
</commit_message>
<xml_diff>
--- a/docs/Getana_Deliverable_2_DailyScrumReport.xlsx
+++ b/docs/Getana_Deliverable_2_DailyScrumReport.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,8 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C58FA5-D1ED-7349-A222-A4174D96A01D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="104">
   <si>
     <t>Daily Scrum Report — Sprint 1</t>
   </si>
@@ -190,9 +191,6 @@
     <t>xx Feb 18</t>
   </si>
   <si>
-    <t>(for this sprint, everyone is on the development team, but this should not be the usual)</t>
-  </si>
-  <si>
     <t>Daily Scrum Report — Sprint 3</t>
   </si>
   <si>
@@ -251,6 +249,96 @@
   </si>
   <si>
     <t>What they will do: Implement front end for route display after API calls to generate route</t>
+  </si>
+  <si>
+    <t>What they will do: Test hashmap functionality</t>
+  </si>
+  <si>
+    <t>What they have done: Completed Android Studio &amp; Google Maps API tutorials, Completed focus group session, Implemented hashmap for building to address mapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they have done: Added Google maps API key to project, Created some basic activites for app, Implemented load/save for schedules </t>
+  </si>
+  <si>
+    <t>What impediments prevent them from progressing: Other classwork</t>
+  </si>
+  <si>
+    <t>What they will do: Complete save/load schedule implementation</t>
+  </si>
+  <si>
+    <t>What they have done: Completed creating home screen, create schedule screen and settings screen and linked those screens with buttons from home screen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What impediments prevent them from progressing: Has been sick. </t>
+  </si>
+  <si>
+    <t>What they will do: Work on user interface</t>
+  </si>
+  <si>
+    <t>What they have done: Completed focus group session</t>
+  </si>
+  <si>
+    <t>What impediments prevent them from progressing: Unfamiliarity with platforms/APIs</t>
+  </si>
+  <si>
+    <t>What impediments prevent them from progressing: Problems with Android Studio</t>
+  </si>
+  <si>
+    <t>What they will do: Continue working on app implementation</t>
+  </si>
+  <si>
+    <t>What they have done: Organized focus group participants, Completed focus group session, Led focus group interaction, Started edit schedule interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they will do: Continue working on app implementation </t>
+  </si>
+  <si>
+    <t>What impediments prevent them from progressing:  Busy schedule/other classwork, Unfamiliarity with platforms/APIs</t>
+  </si>
+  <si>
+    <t>What they have done: Began work on implementing Maps API code calls.</t>
+  </si>
+  <si>
+    <t>What they will do: Complete implementation tasks, Creat configuration management plan document</t>
+  </si>
+  <si>
+    <t>What impediments prevent them from progressing: Difficulty with implementation</t>
+  </si>
+  <si>
+    <t>What they have done: Rewrote hashmap to utilize latitudinal and longitudal coordinates(addresses were not accurate enough)</t>
+  </si>
+  <si>
+    <t>What impediments prevent them from progressing: Difficulty with implementation, other classwork</t>
+  </si>
+  <si>
+    <t>What they have done: Began working on user interface implementation</t>
+  </si>
+  <si>
+    <t>What they have done:  Began working on user interface implementation</t>
+  </si>
+  <si>
+    <t>What they have done: Completed work for saving/loading schedules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they have done: Began working on map interface imlementation </t>
+  </si>
+  <si>
+    <t>What they will do: Update platform &amp; SRS/Use case model document. Create GRL &amp; UCM models document. Complete first app release implementation.</t>
+  </si>
+  <si>
+    <t>What they will do:  Create GRL &amp; UCM models document. Complete first app release implementation.</t>
+  </si>
+  <si>
+    <t>What impediments prevent them from progressing: Difficulty with implementation, other classwork, Still not feeling well</t>
+  </si>
+  <si>
+    <t>What they will do: Update product backlog,Complete first app release implementation. Create domain model &amp; detailed design document.</t>
+  </si>
+  <si>
+    <t>What they will do:Create domain model &amp; detailed design document. Complete first app release implementation.</t>
+  </si>
+  <si>
+    <t>What they will do: Complete sprint 2 and 3 reviews, team member report, &amp; focus group document. Update sprint/product backlog at end of sprint. Complete first app release implementation. Create GRL &amp; UCM models document.</t>
   </si>
 </sst>
 </file>
@@ -1419,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L108"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="125" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView topLeftCell="A38" zoomScale="107" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1442,7 +1530,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -1463,17 +1551,17 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -1481,17 +1569,17 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.15">
@@ -1499,17 +1587,17 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.15">
@@ -1517,17 +1605,17 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.15">
@@ -1535,17 +1623,17 @@
         <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.15">
@@ -1553,17 +1641,17 @@
         <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.15">
@@ -1593,17 +1681,17 @@
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.15">
@@ -1611,17 +1699,17 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.15">
@@ -1629,17 +1717,17 @@
         <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.15">
@@ -1647,17 +1735,17 @@
         <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.15">
@@ -1665,17 +1753,17 @@
         <v>20</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.15">
@@ -1683,17 +1771,17 @@
         <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.15">
@@ -1714,8 +1802,8 @@
       <c r="A59" t="s">
         <v>41</v>
       </c>
-      <c r="B59" t="s">
-        <v>53</v>
+      <c r="B59" s="4">
+        <v>43154</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.15">
@@ -1723,17 +1811,17 @@
         <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C61" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C62" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.15">
@@ -1741,17 +1829,17 @@
         <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C65" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C66" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.15">
@@ -1759,17 +1847,17 @@
         <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C69" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C70" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.15">
@@ -1777,17 +1865,17 @@
         <v>18</v>
       </c>
       <c r="C72" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C73" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C74" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.15">
@@ -1795,17 +1883,17 @@
         <v>20</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C77" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C78" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.15">
@@ -1813,164 +1901,34 @@
         <v>22</v>
       </c>
       <c r="C80" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C81" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.15">
       <c r="C82" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A84" t="s">
-        <v>48</v>
-      </c>
-      <c r="B84" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B85" t="s">
-        <v>7</v>
-      </c>
-      <c r="C85" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C86" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C87" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B89" t="s">
-        <v>13</v>
-      </c>
-      <c r="C89" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C90" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C91" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B93" t="s">
-        <v>16</v>
-      </c>
-      <c r="C93" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C94" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C95" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B97" t="s">
-        <v>18</v>
-      </c>
-      <c r="C97" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C98" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C99" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B101" t="s">
-        <v>20</v>
-      </c>
-      <c r="C101" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C102" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C103" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B105" t="s">
-        <v>22</v>
-      </c>
-      <c r="C105" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C106" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C107" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A108" s="3" t="s">
+      <c r="A83" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3"/>
-      <c r="G108" s="3"/>
-      <c r="H108" s="3"/>
-      <c r="I108" s="3"/>
-      <c r="J108" s="3"/>
-      <c r="K108" s="3"/>
-      <c r="L108" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1984,10 +1942,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L108"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1997,7 +1955,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -2005,545 +1963,537 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>43161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B10" t="s">
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B33" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C11" t="s">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B53" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C54" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C12" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C55" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B14" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C59" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C60" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B62" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C62" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C15" t="s">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C64" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B66" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C67" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C68" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C71" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C72" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B74" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C76" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B78" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C79" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C80" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
+        <v>48</v>
+      </c>
+      <c r="B82" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C84" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C16" t="s">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C85" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B18" t="s">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B87" t="s">
+        <v>13</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C89" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B91" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C19" t="s">
+      <c r="C91" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C92" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C20" t="s">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C93" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B95" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C97" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B99" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C101" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B103" t="s">
+        <v>22</v>
+      </c>
+      <c r="C103" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C104" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C105" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C44" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B47" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C48" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B51" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C52" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C53" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B55" t="s">
-        <v>22</v>
-      </c>
-      <c r="C55" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C56" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C57" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A59" t="s">
-        <v>41</v>
-      </c>
-      <c r="B59" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B60" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C61" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C62" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B64" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C65" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B68" t="s">
-        <v>16</v>
-      </c>
-      <c r="C68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C69" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C70" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B72" t="s">
-        <v>18</v>
-      </c>
-      <c r="C72" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C73" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C74" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B76" t="s">
-        <v>20</v>
-      </c>
-      <c r="C76" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C77" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C78" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B80" t="s">
-        <v>22</v>
-      </c>
-      <c r="C80" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C81" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C82" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A84" t="s">
-        <v>48</v>
-      </c>
-      <c r="B84" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B85" t="s">
-        <v>7</v>
-      </c>
-      <c r="C85" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C86" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C87" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B89" t="s">
-        <v>13</v>
-      </c>
-      <c r="C89" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C90" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C91" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B93" t="s">
-        <v>16</v>
-      </c>
-      <c r="C93" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C94" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C95" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B97" t="s">
-        <v>18</v>
-      </c>
-      <c r="C97" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C98" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C99" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B101" t="s">
-        <v>20</v>
-      </c>
-      <c r="C101" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C102" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C103" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B105" t="s">
-        <v>22</v>
-      </c>
-      <c r="C105" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C106" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="C107" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A108" s="3" t="s">
+      <c r="A106" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3"/>
-      <c r="G108" s="3"/>
-      <c r="H108" s="3"/>
-      <c r="I108" s="3"/>
-      <c r="J108" s="3"/>
-      <c r="K108" s="3"/>
-      <c r="L108" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>